<commit_message>
Removed locale row from spreadsheet.
</commit_message>
<xml_diff>
--- a/config/translations.xlsx
+++ b/config/translations.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="34960" windowHeight="22920"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>en</t>
   </si>
@@ -28,24 +36,6 @@
   </si>
   <si>
     <t>it</t>
-  </si>
-  <si>
-    <t>locale</t>
-  </si>
-  <si>
-    <t>EN</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>DE</t>
-  </si>
-  <si>
-    <t>FR</t>
-  </si>
-  <si>
-    <t>IT</t>
   </si>
   <si>
     <t>h1</t>
@@ -159,23 +149,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -194,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -254,180 +231,99 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="001FB714"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -629,7 +525,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -648,7 +544,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -678,7 +574,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -704,7 +600,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -730,7 +626,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -756,7 +652,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -782,7 +678,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -808,7 +704,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -834,7 +730,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -860,7 +756,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -886,7 +782,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -899,9 +795,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -918,7 +820,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -937,7 +839,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -963,7 +865,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -989,7 +891,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1015,7 +917,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1041,7 +943,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1067,7 +969,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1093,7 +995,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1119,7 +1021,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1145,7 +1047,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1171,7 +1073,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1184,9 +1086,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1200,7 +1108,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1219,7 +1127,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1249,7 +1157,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1275,7 +1183,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1301,7 +1209,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1327,7 +1235,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1353,7 +1261,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1379,7 +1287,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1405,7 +1313,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1431,7 +1339,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1457,7 +1365,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1470,304 +1378,267 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1719" style="1" customWidth="1"/>
-    <col min="7" max="256" width="8.85156" style="1" customWidth="1"/>
+    <col min="4" max="6" width="15.1640625" style="1" customWidth="1"/>
+    <col min="7" max="256" width="8.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s" s="6">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="3">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s" s="5">
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s" s="6">
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="3">
+    <row r="4" spans="1:6" ht="15" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s" s="3">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s" s="3">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s" s="3">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="3">
+    <row r="5" spans="1:6" ht="15" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s" s="3">
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s" s="3">
+      <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s" s="3">
+      <c r="E5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s" s="3">
+      <c r="F5" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="3">
+    <row r="6" spans="1:6" ht="15" customHeight="1">
+      <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s" s="3">
+      <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s" s="3">
+      <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s" s="3">
+      <c r="D6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s" s="3">
+      <c r="E6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F6" t="s" s="3">
+      <c r="F6" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="3">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s" s="3">
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s" s="3">
+      <c r="C7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D7" t="s" s="3">
+      <c r="D7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s" s="3">
+      <c r="E7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F7" t="s" s="3">
+      <c r="F7" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s" s="3">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="E8" t="s" s="3">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s" s="3">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="16" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="16" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="16" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="16" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="16" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="16" customWidth="1"/>
+    <col min="1" max="256" width="8.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1776,93 +1647,93 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="17" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="17" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="17" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="17" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="17" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="17" customWidth="1"/>
+    <col min="1" max="256" width="8.83203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1871,9 +1742,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>